<commit_message>
Added UI Section to Design Document
</commit_message>
<xml_diff>
--- a/Trimester One/Documentation/Report/Project Management.xlsx
+++ b/Trimester One/Documentation/Report/Project Management.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b00330023\Desktop\y3-games-dev-project-master\Trimester One\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasd\Documents\Unity\Projects\Version Control\y3-games-dev-project\Trimester One\Documentation\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F7673-B561-4533-B99E-445158763FC9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
     <sheet name="Checklist" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
   <si>
     <t>30th Nov. (DEADLINE)</t>
   </si>
@@ -274,12 +280,15 @@
   </si>
   <si>
     <t>Trimester One</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -553,9 +562,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -573,9 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,6 +598,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1017,11 +1026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1303,7 @@
       <c r="N10" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -1335,12 +1344,12 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="41"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1352,11 +1361,11 @@
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1369,7 +1378,7 @@
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="33" t="s">
         <v>74</v>
       </c>
       <c r="B15" s="21"/>
@@ -1386,7 +1395,7 @@
       <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B16" s="21"/>
@@ -1403,7 +1412,7 @@
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="21"/>
@@ -1420,11 +1429,11 @@
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="11"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -1437,7 +1446,7 @@
       <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="33" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="21"/>
@@ -1454,12 +1463,12 @@
       <c r="M19" s="15"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="34" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="37"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -1468,7 +1477,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="42"/>
+      <c r="M20" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,618 +1486,613 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="5" width="19" style="28" customWidth="1"/>
+    <col min="3" max="5" width="19" style="27" customWidth="1"/>
     <col min="7" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="31" t="str">
+      <c r="B2" s="41"/>
+      <c r="C2" s="30" t="str">
         <f>IF(COUNTIF(C3:C8, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D2" s="31" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D2" s="30" t="str">
         <f>IF(COUNTIF(D3:D8, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="E2" s="33">
+        <v>Yes</v>
+      </c>
+      <c r="E2" s="31">
         <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="29"/>
+      <c r="C3" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="29"/>
+      <c r="C4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="C5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="29"/>
+      <c r="C6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="29"/>
+      <c r="C7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="29"/>
+      <c r="C8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31" t="str">
-        <f>IF(COUNTIF(C10:C12, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D9" s="31" t="str">
-        <f>IF(COUNTIF(D10:D12, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="E9" s="33">
+      <c r="B9" s="41"/>
+      <c r="C9" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="31">
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="29"/>
+      <c r="C10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="29"/>
+      <c r="C11" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="29"/>
+      <c r="C12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="31" t="str">
+      <c r="B13" s="41"/>
+      <c r="C13" s="30" t="str">
         <f>IF(COUNTIF(C14:C21, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D13" s="31" t="str">
-        <f>IF(COUNTIF(D14:D21, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="E13" s="33">
+        <v>Yes</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="29"/>
+      <c r="C14" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="29"/>
+      <c r="C15" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="29"/>
+      <c r="C16" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="26" t="s">
+      <c r="A17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="29"/>
+      <c r="C17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="29"/>
+      <c r="C18" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="29"/>
+      <c r="C19" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="29"/>
+      <c r="C20" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="29"/>
+      <c r="C21" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="31" t="str">
+      <c r="B22" s="41"/>
+      <c r="C22" s="30" t="str">
         <f>IF(COUNTIF(C23:C30, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D22" s="31" t="str">
-        <f>IF(COUNTIF(D23:D30, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="E22" s="33">
+        <v>Yes</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="31">
         <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="29"/>
+      <c r="C23" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="29"/>
+      <c r="C24" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="29"/>
+      <c r="C25" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="29"/>
+      <c r="C26" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="29"/>
+      <c r="C27" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="29"/>
+      <c r="C28" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="29"/>
+      <c r="C29" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="29"/>
+      <c r="C30" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="31" t="str">
+      <c r="B31" s="41"/>
+      <c r="C31" s="30" t="str">
         <f>IF(COUNTIF(C32:C34, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D31" s="31" t="str">
-        <f>IF(COUNTIF(D32:D34, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="E31" s="33">
+        <v>Yes</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="31">
         <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="26" t="s">
+      <c r="A32" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="29"/>
+      <c r="C32" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="26" t="s">
+      <c r="A33" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="29"/>
+      <c r="C33" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="28"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="26" t="s">
+      <c r="A34" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="29"/>
+      <c r="C34" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="31" t="str">
+      <c r="B35" s="41"/>
+      <c r="C35" s="30" t="str">
         <f>IF(COUNTIF(C36:C39, "&lt;&gt;Yes")=0, "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="D35" s="31" t="str">
+      <c r="D35" s="30" t="str">
         <f>IF(COUNTIF(D36:D39, "&lt;&gt;Yes")=0, "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="31">
         <v>0.1</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="26" t="s">
+      <c r="A37" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="26" t="s">
+      <c r="A38" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="28"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Added Critical Appraisal To Design Document
+ Added the Meeting Minutes document to the repository as it was previously stored locally.
</commit_message>
<xml_diff>
--- a/Trimester One/Documentation/Report/Project Management.xlsx
+++ b/Trimester One/Documentation/Report/Project Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasd\Documents\Unity\Projects\Version Control\y3-games-dev-project\Trimester One\Documentation\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F7673-B561-4533-B99E-445158763FC9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB9407-1621-4260-B1D7-F498F6418C64}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="83">
   <si>
     <t>30th Nov. (DEADLINE)</t>
   </si>
@@ -220,9 +221,6 @@
   </si>
   <si>
     <t>UI Sketch (Menu &amp; Game)</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Technical Approach</t>
@@ -1029,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1040,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>19</v>
@@ -1229,8 +1227,8 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="15"/>
@@ -1304,7 +1302,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>19</v>
@@ -1345,7 +1343,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -1362,7 +1360,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -1379,7 +1377,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1396,7 +1394,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -1413,7 +1411,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -1430,7 +1428,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -1447,7 +1445,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -1464,7 +1462,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -1489,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,10 +1539,10 @@
         <v>38</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="28"/>
     </row>
@@ -1556,10 +1554,10 @@
         <v>39</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="28"/>
     </row>
@@ -1571,10 +1569,10 @@
         <v>40</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="28"/>
     </row>
@@ -1586,10 +1584,10 @@
         <v>41</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="28"/>
     </row>
@@ -1601,10 +1599,10 @@
         <v>42</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="28"/>
     </row>
@@ -1616,10 +1614,10 @@
         <v>43</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="28"/>
     </row>
@@ -1629,10 +1627,10 @@
       </c>
       <c r="B9" s="41"/>
       <c r="C9" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="31">
         <v>0.1</v>
@@ -1646,10 +1644,10 @@
         <v>45</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="28"/>
     </row>
@@ -1661,10 +1659,10 @@
         <v>46</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="28"/>
     </row>
@@ -1676,10 +1674,10 @@
         <v>47</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="28"/>
     </row>
@@ -1693,7 +1691,7 @@
         <v>Yes</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="31">
         <v>0.25</v>
@@ -1707,10 +1705,10 @@
         <v>48</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="28"/>
     </row>
@@ -1722,10 +1720,10 @@
         <v>49</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="28"/>
     </row>
@@ -1737,10 +1735,10 @@
         <v>50</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="28"/>
     </row>
@@ -1752,10 +1750,10 @@
         <v>51</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="28"/>
     </row>
@@ -1767,10 +1765,10 @@
         <v>52</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="28"/>
     </row>
@@ -1782,10 +1780,10 @@
         <v>54</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19" s="28"/>
     </row>
@@ -1797,10 +1795,10 @@
         <v>53</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="28"/>
     </row>
@@ -1812,10 +1810,10 @@
         <v>55</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="28"/>
     </row>
@@ -1829,7 +1827,7 @@
         <v>Yes</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="31">
         <v>0.2</v>
@@ -1840,13 +1838,13 @@
         <v>44</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="28"/>
     </row>
@@ -1858,10 +1856,10 @@
         <v>56</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E24" s="28"/>
     </row>
@@ -1873,10 +1871,10 @@
         <v>57</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="28"/>
     </row>
@@ -1888,10 +1886,10 @@
         <v>58</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="28"/>
     </row>
@@ -1903,10 +1901,10 @@
         <v>60</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="28"/>
     </row>
@@ -1918,10 +1916,10 @@
         <v>59</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28" s="28"/>
     </row>
@@ -1933,10 +1931,10 @@
         <v>61</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E29" s="28"/>
     </row>
@@ -1948,10 +1946,10 @@
         <v>62</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="28"/>
     </row>
@@ -1965,7 +1963,7 @@
         <v>Yes</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="31">
         <v>0.3</v>
@@ -1976,13 +1974,13 @@
         <v>44</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="28"/>
     </row>
@@ -1991,13 +1989,13 @@
         <v>44</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E33" s="28"/>
     </row>
@@ -2006,28 +2004,27 @@
         <v>44</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="30" t="str">
         <f>IF(COUNTIF(C36:C39, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D35" s="30" t="str">
-        <f>IF(COUNTIF(D36:D39, "&lt;&gt;Yes")=0, "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="E35" s="31">
         <v>0.1</v>
@@ -2039,13 +2036,13 @@
         <v>44</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E36" s="28"/>
     </row>
@@ -2054,13 +2051,13 @@
         <v>44</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E37" s="28"/>
     </row>
@@ -2069,13 +2066,13 @@
         <v>44</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E38" s="28"/>
     </row>
@@ -2084,13 +2081,13 @@
         <v>44</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E39" s="28"/>
     </row>

</xml_diff>